<commit_message>
added more data Pog
</commit_message>
<xml_diff>
--- a/results/distances.xlsx
+++ b/results/distances.xlsx
@@ -41,7 +41,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-All Values present in this excel sheet represent the average of ten iterations</t>
+All values present in this excel sheet represent the average of ten iterations</t>
         </r>
       </text>
     </comment>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>KDD17</t>
   </si>
@@ -61,44 +61,95 @@
     <t>EconomyNews</t>
   </si>
   <si>
+    <t>0.5793 (±0.02103)</t>
+  </si>
+  <si>
+    <t>-0.8304 (±0.01109)</t>
+  </si>
+  <si>
+    <t>1.9173 (±0.00757)</t>
+  </si>
+  <si>
+    <t>-1.0409 (±0.04034)</t>
+  </si>
+  <si>
+    <t>1.7979 (±0.01644)</t>
+  </si>
+  <si>
+    <t>-1.6018 (±0.08220)</t>
+  </si>
+  <si>
     <t>Phrasebank</t>
   </si>
   <si>
-    <t>0.5793 (±0.02103)</t>
-  </si>
-  <si>
-    <t>-0.8304 (±0.01109)</t>
-  </si>
-  <si>
-    <t>1.9173 (±0.00757)</t>
-  </si>
-  <si>
-    <t>-1.0409 (±0.04034)</t>
-  </si>
-  <si>
-    <t>1.7979 (±0.01644)</t>
-  </si>
-  <si>
-    <t>1.7489 (±0.01311)</t>
-  </si>
-  <si>
-    <t>1.8656 (±0.00707)</t>
-  </si>
-  <si>
-    <t>PhrasebankAllAgree</t>
-  </si>
-  <si>
-    <t>1.9211 (±000606)</t>
-  </si>
-  <si>
-    <t>1.8139(±0.01599)</t>
+    <t>1.8697 (±0.00956)</t>
+  </si>
+  <si>
+    <t>1.7443 (±0.01189)</t>
+  </si>
+  <si>
+    <t>1.7978 (±0.03142)</t>
+  </si>
+  <si>
+    <t>-1.4674 (±0.019566)</t>
+  </si>
+  <si>
+    <t>BBCSport</t>
+  </si>
+  <si>
+    <t>1.9182 (±0.00754)</t>
+  </si>
+  <si>
+    <t>1.8839 (±0.01401)</t>
+  </si>
+  <si>
+    <t>1.8871 (±0.01388)</t>
+  </si>
+  <si>
+    <t>1.7842 (±0.01275)</t>
+  </si>
+  <si>
+    <t>-1.4021 (±0.02795)</t>
+  </si>
+  <si>
+    <t>SLSAmazon</t>
+  </si>
+  <si>
+    <t>1.9646 (±0.00397)</t>
+  </si>
+  <si>
+    <t>1.9295 (±0.01568)</t>
+  </si>
+  <si>
+    <t>1.8914 (±0.02574)</t>
+  </si>
+  <si>
+    <t>1.8844 (±0.00978)</t>
+  </si>
+  <si>
+    <t>1.7804 (±0.03478)</t>
+  </si>
+  <si>
+    <t>-1.5290 (±0.06082)</t>
+  </si>
+  <si>
+    <t>SLSIMBD</t>
+  </si>
+  <si>
+    <t>1(±1)</t>
+  </si>
+  <si>
+    <t>1.9658 (±0.00492)</t>
+  </si>
+  <si>
+    <t>1.9337(±0.01045)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +185,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +223,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,82 +518,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="D8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started to add more distances
</commit_message>
<xml_diff>
--- a/results/distances.xlsx
+++ b/results/distances.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
   <si>
     <t>KDD17</t>
   </si>
@@ -136,13 +136,91 @@
     <t>SLSIMBD</t>
   </si>
   <si>
-    <t>1(±1)</t>
-  </si>
-  <si>
     <t>1.9658 (±0.00492)</t>
   </si>
   <si>
     <t>1.9337(±0.01045)</t>
+  </si>
+  <si>
+    <t>1.9337 (±0.01045)</t>
+  </si>
+  <si>
+    <t>1.8965 (±0.03098)</t>
+  </si>
+  <si>
+    <t>1.8998 (±0.01852)</t>
+  </si>
+  <si>
+    <t>1.7451 (±0.02679)</t>
+  </si>
+  <si>
+    <t>1.3460 (±0.07877)</t>
+  </si>
+  <si>
+    <t>-1.5820 (±0.04367)</t>
+  </si>
+  <si>
+    <t>SLSYelp</t>
+  </si>
+  <si>
+    <t>1.9736 (±0.00372)</t>
+  </si>
+  <si>
+    <t>1.9443 (±0.00845)</t>
+  </si>
+  <si>
+    <t>1.9105 (±0.03012)</t>
+  </si>
+  <si>
+    <t>1.8998 (±0.01094)</t>
+  </si>
+  <si>
+    <t>1.7608 (±0.01885)</t>
+  </si>
+  <si>
+    <t>1.2920 (±0.10891)</t>
+  </si>
+  <si>
+    <t>1.4260 (±0.06204)</t>
+  </si>
+  <si>
+    <t>-1.5870 (±0.05438)</t>
+  </si>
+  <si>
+    <t>STSGold</t>
+  </si>
+  <si>
+    <t>1.9604 (±0.00508)</t>
+  </si>
+  <si>
+    <t>1.9460 (±0.00672)</t>
+  </si>
+  <si>
+    <t>1.9292 (±0.02288)</t>
+  </si>
+  <si>
+    <t>1.9299 (±0.00649)</t>
+  </si>
+  <si>
+    <t>1.6766 (±0.02538)</t>
+  </si>
+  <si>
+    <t>1.6633 (±0.05061)</t>
+  </si>
+  <si>
+    <t>1.6850 (±0.03915)</t>
+  </si>
+  <si>
+    <t>1.5941 (±0.02867)</t>
+  </si>
+  <si>
+    <t>-1.5553 (±0.02868)</t>
+  </si>
+  <si>
+    <t>PAD</t>
+  </si>
+  <si>
+    <t>-121.3429</t>
   </si>
 </sst>
 </file>
@@ -186,10 +264,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +303,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="D8:G8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -529,13 +611,18 @@
     <col min="1" max="1" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="33.75">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,8 +644,14 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -581,10 +674,16 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -606,8 +705,17 @@
       <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -629,8 +737,17 @@
       <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -652,8 +769,17 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -675,8 +801,17 @@
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -698,28 +833,195 @@
       <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>28</v>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="33.75">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all four distances
</commit_message>
<xml_diff>
--- a/results/distances.xlsx
+++ b/results/distances.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="113">
   <si>
     <t>KDD17</t>
   </si>
@@ -220,7 +220,175 @@
     <t>PAD</t>
   </si>
   <si>
-    <t>-121.3429</t>
+    <t>-121.6129</t>
+  </si>
+  <si>
+    <t>-1.9393</t>
+  </si>
+  <si>
+    <t>-3.5350</t>
+  </si>
+  <si>
+    <t>-121.2823</t>
+  </si>
+  <si>
+    <t>-13.2600</t>
+  </si>
+  <si>
+    <t>-97.3825</t>
+  </si>
+  <si>
+    <t>-119.0565</t>
+  </si>
+  <si>
+    <t>-125.2258</t>
+  </si>
+  <si>
+    <t>-125.1508</t>
+  </si>
+  <si>
+    <t>-100.8900</t>
+  </si>
+  <si>
+    <t>-127.5615</t>
+  </si>
+  <si>
+    <t>-100.8800</t>
+  </si>
+  <si>
+    <t>Kl Distance</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1082.1677</t>
+  </si>
+  <si>
+    <t>1075.8788</t>
+  </si>
+  <si>
+    <t>531.7172</t>
+  </si>
+  <si>
+    <t>Hellinger Distance</t>
+  </si>
+  <si>
+    <t>395.7386</t>
+  </si>
+  <si>
+    <t>357.1053</t>
+  </si>
+  <si>
+    <t>Total Variation Distance</t>
+  </si>
+  <si>
+    <t>5030460.0000</t>
+  </si>
+  <si>
+    <t>5049967.5000</t>
+  </si>
+  <si>
+    <t>4855509.5000</t>
+  </si>
+  <si>
+    <t>5032040.5000</t>
+  </si>
+  <si>
+    <t>5065724.0000</t>
+  </si>
+  <si>
+    <t>5043882.5000</t>
+  </si>
+  <si>
+    <t>5043416.5000</t>
+  </si>
+  <si>
+    <t>5041835.5000</t>
+  </si>
+  <si>
+    <t>1320839.1250</t>
+  </si>
+  <si>
+    <t>1326449.6250</t>
+  </si>
+  <si>
+    <t>1357866.7500</t>
+  </si>
+  <si>
+    <t>1336782.8750</t>
+  </si>
+  <si>
+    <t>1334579.8750</t>
+  </si>
+  <si>
+    <t>1341450.1250</t>
+  </si>
+  <si>
+    <t>1339776.6250</t>
+  </si>
+  <si>
+    <t>793505.6875</t>
+  </si>
+  <si>
+    <t>676578.9375</t>
+  </si>
+  <si>
+    <t>167361.4219</t>
+  </si>
+  <si>
+    <t>165450.4688</t>
+  </si>
+  <si>
+    <t>170107.7188</t>
+  </si>
+  <si>
+    <t>330099.9375</t>
+  </si>
+  <si>
+    <t>839007.6250</t>
+  </si>
+  <si>
+    <t>812056.0625</t>
+  </si>
+  <si>
+    <t>810975.9375</t>
+  </si>
+  <si>
+    <t>815870.5000</t>
+  </si>
+  <si>
+    <t>814918.6250</t>
+  </si>
+  <si>
+    <t>693579.8125</t>
+  </si>
+  <si>
+    <t>688462.6875</t>
+  </si>
+  <si>
+    <t>693111.3125</t>
+  </si>
+  <si>
+    <t>688199.5625</t>
+  </si>
+  <si>
+    <t>165885.2969</t>
+  </si>
+  <si>
+    <t>167481.8125</t>
+  </si>
+  <si>
+    <t>333478.9375</t>
+  </si>
+  <si>
+    <t>164795.1719</t>
+  </si>
+  <si>
+    <t>331628.9375</t>
+  </si>
+  <si>
+    <t>334233.7813</t>
   </si>
 </sst>
 </file>
@@ -600,15 +768,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
@@ -940,7 +1108,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="33.75">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -976,52 +1146,925 @@
       <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="C13" s="1">
+        <v>-101.10720000000001</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-99.164599999999993</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-98.68</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-97.527299999999997</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-97.542199999999994</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-97.518699999999995</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-97.918599999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="1">
+        <v>-29.7789</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-98.081999999999994</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-104.691</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-102.8927</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-98.585400000000007</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-98.675200000000004</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-98.5809</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-99.941199999999995</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-7.2793999999999999</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-12.7254</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-14.757300000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-60.058900000000001</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-60.666699999999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-60.3645</v>
+      </c>
+      <c r="J15" s="1">
+        <v>-29.650400000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="B16" s="1">
+        <v>-16.998799999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-63.8735</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-100.12009999999999</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-108.2688</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-101.0184</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-100.91240000000001</v>
+      </c>
+      <c r="J16" s="1">
+        <v>-103.3051</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="B17" s="1">
+        <v>-14.137700000000001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-53.145800000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-99.639799999999994</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-92.628399999999999</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-100.57689999999999</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-100.7689</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-103.82689999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="B18" s="1">
+        <v>-3.5539000000000001</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-13.315099999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-107.0254</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-23.1629</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-27.165500000000002</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="1">
+        <v>-114.1863</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-114.29340000000001</v>
+      </c>
+      <c r="J18" s="1">
+        <v>-55.732799999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="B19" s="1">
+        <v>-3.5308999999999999</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-106.3638</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-23.027100000000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-27.150200000000002</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-112.9405</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-127.18049999999999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-113.8473</v>
+      </c>
+      <c r="J19" s="1">
+        <v>-55.476799999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-13.2699</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-106.94119999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>-23.1099</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-27.263200000000001</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-113.9619</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-114.74720000000001</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-128.78870000000001</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-55.880200000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-7.1101000000000001</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-26.600899999999999</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-102.4361</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-46.393900000000002</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-55.021099999999997</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-105.4451</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-105.78579999999999</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-105.75020000000001</v>
+      </c>
+      <c r="J21" s="1">
+        <v>-125.02630000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="33.75">
+      <c r="A23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="1">
+        <v>957.97220000000004</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1017.1606</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1029.3415</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1075.7989</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1075.8432</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1060.4818</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <v>957.97220000000004</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1">
+        <v>544.00530000000003</v>
+      </c>
+      <c r="E25" s="1">
+        <v>402.74250000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>432.20240000000001</v>
+      </c>
+      <c r="G25" s="1">
+        <v>531.67920000000004</v>
+      </c>
+      <c r="H25" s="1">
+        <v>531.71720000000005</v>
+      </c>
+      <c r="I25" s="1">
+        <v>531.79520000000002</v>
+      </c>
+      <c r="J25" s="1">
+        <v>501.2758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1">
+        <v>544.00530000000003</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="1">
+        <v>412.88170000000002</v>
+      </c>
+      <c r="F26" s="1">
+        <v>376.52569999999997</v>
+      </c>
+      <c r="G26" s="1">
+        <v>143.9692</v>
+      </c>
+      <c r="H26" s="1">
+        <v>144.41679999999999</v>
+      </c>
+      <c r="I26" s="1">
+        <v>145.5829</v>
+      </c>
+      <c r="J26" s="1">
+        <v>245.1798</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1017.1606</v>
+      </c>
+      <c r="C27" s="1">
+        <v>402.74250000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>412.88170000000002</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="1">
+        <v>234.274</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="1">
+        <v>395.76280000000003</v>
+      </c>
+      <c r="I27" s="1">
+        <v>395.8168</v>
+      </c>
+      <c r="J27" s="1">
+        <v>351.0521</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1029.3415</v>
+      </c>
+      <c r="C28" s="1">
+        <v>432.20240000000001</v>
+      </c>
+      <c r="D28" s="1">
+        <v>376.52569999999997</v>
+      </c>
+      <c r="E28" s="1">
+        <v>234.274</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="1">
+        <v>357.21109999999999</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="1">
+        <v>357.27730000000003</v>
+      </c>
+      <c r="J28" s="1">
+        <v>305.0942</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1075.7989</v>
+      </c>
+      <c r="C29" s="1">
+        <v>531.67920000000004</v>
+      </c>
+      <c r="D29" s="1">
+        <v>143.9692</v>
+      </c>
+      <c r="E29" s="1">
+        <v>395.73860000000002</v>
+      </c>
+      <c r="F29" s="1">
+        <v>357.21109999999999</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="1">
+        <v>79.209000000000003</v>
+      </c>
+      <c r="I29" s="1">
+        <v>79.463700000000003</v>
+      </c>
+      <c r="J29" s="1">
+        <v>214.33959999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1075.8432</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="1">
+        <v>144.41679999999999</v>
+      </c>
+      <c r="E30" s="1">
+        <v>395.76280000000003</v>
+      </c>
+      <c r="F30" s="1">
+        <v>357.1053</v>
+      </c>
+      <c r="G30" s="1">
+        <v>79.209000000000003</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" s="1">
+        <v>79.075400000000002</v>
+      </c>
+      <c r="J30" s="1">
+        <v>214.2398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1">
+        <v>531.79520000000002</v>
+      </c>
+      <c r="D31" s="1">
+        <v>145.5829</v>
+      </c>
+      <c r="E31" s="1">
+        <v>395.8168</v>
+      </c>
+      <c r="F31" s="1">
+        <v>357.27730000000003</v>
+      </c>
+      <c r="G31" s="1">
+        <v>79.463700000000003</v>
+      </c>
+      <c r="H31" s="1">
+        <v>79.075400000000002</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="1">
+        <v>214.43020000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1060.4818</v>
+      </c>
+      <c r="C32" s="1">
+        <v>501.2758</v>
+      </c>
+      <c r="D32" s="1">
+        <v>245.1798</v>
+      </c>
+      <c r="E32" s="1">
+        <v>351.0521</v>
+      </c>
+      <c r="F32" s="1">
+        <v>305.0942</v>
+      </c>
+      <c r="G32" s="1">
+        <v>214.33959999999999</v>
+      </c>
+      <c r="H32" s="1">
+        <v>214.2398</v>
+      </c>
+      <c r="I32" s="1">
+        <v>214.43020000000001</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="33.75">
+      <c r="A34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>